<commit_message>
updated tamil wittier link
</commit_message>
<xml_diff>
--- a/availabilities2.xlsx
+++ b/availabilities2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b7a8b95bb4fcfbb0/Desktop/Drone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{719EB42A-9DCC-4CB7-B3F8-FFFECE135745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C48D1A0E-EE80-47A4-A421-BC14298EF9A5}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="8_{719EB42A-9DCC-4CB7-B3F8-FFFECE135745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AC01921-DDC4-4BE8-A87D-C73C704E9065}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E5FF2DF9-F760-4A4C-99BE-A9020D00C310}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" xr2:uid="{E5FF2DF9-F760-4A4C-99BE-A9020D00C310}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="116">
   <si>
     <t>SNO</t>
   </si>
@@ -632,14 +632,110 @@
     <t>Conclusion</t>
   </si>
   <si>
-    <t>More costlier than I expected :((</t>
+    <t>More costlier than I expected :(( around  1L</t>
+  </si>
+  <si>
+    <t>Parts</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Frame cinewhoop</t>
+  </si>
+  <si>
+    <t>Basic parts need to fly</t>
+  </si>
+  <si>
+    <t>https://www.quadkart.in/cloud-149-v2-3-inch-cinewhoop-frame-kit/</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://robu.in/product/radiomaster-tx12-mkii-expresslrs-edgetx-radio-controller/?gad_source=1&amp;gclid=Cj0KCQiAkKqsBhC3ARIsAEEjuJixrn-eq08sVZbY3zt8EQqFXp9a1I-jRgZi-mWJpKQS8F4uV-jFaN8aAozqEALw_wcB</t>
+  </si>
+  <si>
+    <t>Radio Transmitter with receiver and battery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motors (4) </t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=QC-36Wfo0q4&amp;list=PL_3XHkWVmS0L8qJ9UAu_fURkJFw8aD5k4&amp;ab_channel=Techwittier-%E0%AE%A4%E0%AE%AE%E0%AE%BF%E0%AE%B4%E0%AF%8D</t>
+  </si>
+  <si>
+    <t>https://www.drkstore.in/geprc-speedx2-1804-2450kv-3450kv-motor/</t>
+  </si>
+  <si>
+    <t>Stack FC and ESC</t>
+  </si>
+  <si>
+    <t>https://robu.in/product/f405-v1-0-flight-controller35a-2-6s-4-in-1-esc-flytower-mpu6000/?gad_source=1&amp;gclid=Cj0KCQiAkKqsBhC3ARIsAEEjuJhtR27vIpTiLYbx6qre8xGnVikIKVSYDwGblV5JkCGVrV9qIF6jxEwaAsWsEALw_wcB</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Drone</t>
+  </si>
+  <si>
+    <t>Batteries</t>
+  </si>
+  <si>
+    <t>1300mAh 4s 120C (4)</t>
+  </si>
+  <si>
+    <t>Charger</t>
+  </si>
+  <si>
+    <t>https://www.quadkart.in/tattu-r-line-version-3-0-1300mah-4s-120c-lipo-battery/</t>
+  </si>
+  <si>
+    <t>https://www.drkstore.in/skyrc-b6-neo-200w-dc-smart-charger-with-dc-pd-dual-input/</t>
+  </si>
+  <si>
+    <t>To add FPV into above</t>
+  </si>
+  <si>
+    <t>VTX</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>Goggles</t>
+  </si>
+  <si>
+    <t>SkyRC B6 Neo 200W - out of stock</t>
+  </si>
+  <si>
+    <t>https://www.quadkopters.com/product/fpv-kit-and-accessories/akk-race-ranger-vtx/</t>
+  </si>
+  <si>
+    <t>AKK Race Ranger VTX</t>
+  </si>
+  <si>
+    <t>https://robu.in/product/1-3-cmos-1500tvl-mini-fpv-camera-2-1mm-lens-pal-ntsc-with-osd/?gad_source=1&amp;gclid=Cj0KCQiAkKqsBhC3ARIsAEEjuJh54Do8gbQ3zbHc6cWJ9_yUoc6Y-iCCvXei-JtfoILL0ASURxYIA4QaAnadEALw_wcB</t>
+  </si>
+  <si>
+    <t>1/3″ CMOS 1500TVL Mini FPV Camera 2.1mm Lens PAL / NTSC With OSD</t>
+  </si>
+  <si>
+    <t>betafpv cetus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -698,6 +794,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -877,66 +981,79 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -965,6 +1082,10 @@
 </file>
 
 <file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1265,21 +1386,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCAA637-03B3-4845-9AD9-8685199D6BB5}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="5"/>
+    <col min="2" max="2" width="40" style="5" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="5"/>
+    <col min="8" max="8" width="26.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -1309,427 +1433,589 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="7">
         <v>3700</v>
       </c>
-      <c r="H2" s="8"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="7">
         <v>10640</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="7">
         <v>7000</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="H4" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="7">
         <v>0</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="7">
         <v>0</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="7">
         <v>0</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="11" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="7">
         <v>15000</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="7">
         <v>0</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="7">
         <v>15000</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="7">
         <v>400</v>
       </c>
-      <c r="H11" s="8"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="7">
         <v>6300</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="H12" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="7">
         <v>3500</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="7">
         <v>0</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12">
+      <c r="A15" s="15">
         <v>14</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="16">
         <v>0</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="18" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="16">
+      <c r="A16" s="19">
         <v>15</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="21">
         <v>27000</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="23" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="5" t="s">
         <v>83</v>
       </c>
     </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="5">
+        <v>14000</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="5">
+        <v>4000</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="24"/>
+      <c r="B35" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="5">
+        <v>6000</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="24"/>
+      <c r="B36" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="5">
+        <v>6400</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" s="5">
+        <v>10000</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="5">
+        <v>3500</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="5">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="5">
+        <v>2200</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="5">
+        <v>1500</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" s="5">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="5">
+        <v>65000</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A34:A36"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1" display="https://www.youtube.com/redirect?event=video_description&amp;redir_token=QUFFLUhqa0tvYi1QR09FZUdoU3hMMVFpeXQwVG16VFdpd3xBQ3Jtc0ttcTE1dl9HM1RGSHlWaldIdi0wSEZ6Um44a01VRUtkYkdrN1Q0WlVNWVJQTUdPMjBmLXhwVC1rVlhNSmJ2eGExNXVtRWtKcGxFRlBlS3o5Rl8tZG1UUUstWURnS1lwN0t6WW1tZENmQ05Ka2dPZ2owTQ&amp;q=https%3A%2F%2Fbit.ly%2F3Q8ysYv&amp;v=ZaBlsTkxKIM" xr:uid="{9B184F22-7BB0-40F8-A333-717CCADF318F}"/>

</xml_diff>